<commit_message>
Added the completed review report for Requirements and Architecture phases.
</commit_message>
<xml_diff>
--- a/Tasks/Docs/CheckListsAll/Lab01_ReviewReport.xlsx
+++ b/Tasks/Docs/CheckListsAll/Lab01_ReviewReport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9875" tabRatio="650"/>
+    <workbookView windowWidth="22943" windowHeight="9875" tabRatio="650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
   <si>
     <t>do not print this form</t>
   </si>
@@ -70,6 +70,9 @@
     <t xml:space="preserve">Review date: </t>
   </si>
   <si>
+    <t>18-03-2020</t>
+  </si>
+  <si>
     <t>Crt. No.</t>
   </si>
   <si>
@@ -82,6 +85,54 @@
     <t>Comments/ improvements</t>
   </si>
   <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>page 1</t>
+  </si>
+  <si>
+    <t>Requirements are partially incomplete regarding what kind of details are displayed for tasks, how is a task displayed in a period filtering, who is actually the user.</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>Requirements are partially missing related to data storage, application interface, programming language.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>Nothing wrong.</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>The initialization of the system has not been considered at all.</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>Although the funtions have been defined, they lack the ammount needed for an atctual implementation.</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>None of the users's needs are stated at all. They must be added.</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>No information about the nevironment is given.</t>
+  </si>
+  <si>
     <t>Effort to review document (hours):</t>
   </si>
   <si>
@@ -95,6 +146,66 @@
   </si>
   <si>
     <t>Georgescu Anca</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>diagram.uml</t>
+  </si>
+  <si>
+    <t>Many connection are missing between Service, Repository and Domain.There are service methods scattered in other classes two, bad practice.</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>It's not consistent, at the first glance it seems a normal MVC project, but Services package doesn't fit in the architecture. Files must be moved.A better choice considering the situation would be a Domain-Repo-Service-Controller arhitectur. Many files must be moved from a category to another.</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>Yes, mostly</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>Mostly yes, but in the case of TaskList ( which is an interface ) it has two implementation. One is used everywhere and the other one only in a specific method with no apparent advantages.</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Yes, using log error</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>Using exception logging and observer.</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>The names are mostly intuitively except a couple : TaskIO ( instead of TaskRepository ), TaskOperation ( better TaskFilter ). NO description is provided for any of the clasess, they must be added.</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>THERE ARE NO DESCRIPTIONS.</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>A10</t>
   </si>
   <si>
     <t>Review Form. Coding Defects</t>
@@ -1294,8 +1405,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4"/>
@@ -1388,91 +1499,140 @@
       <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="3:5">
       <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="10"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" ht="57.6" spans="2:5">
       <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" ht="43.2" spans="2:6">
       <c r="B11" s="6">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="C11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="6">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" ht="28.8" spans="2:5">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="2:5">
+      <c r="C13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" ht="43.2" spans="2:5">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="2:5">
+      <c r="C14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" ht="28.8" spans="2:5">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
+      <c r="C15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
+      <c r="C16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="6">
@@ -1560,7 +1720,7 @@
     </row>
     <row r="27" spans="3:5">
       <c r="C27" s="21" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="13"/>
@@ -1587,8 +1747,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4"/>
@@ -1615,7 +1775,7 @@
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1644,7 +1804,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E4" s="24"/>
       <c r="H4" s="6" t="s">
@@ -1659,10 +1819,10 @@
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="23" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E5" s="26"/>
       <c r="H5" s="6" t="s">
@@ -1680,118 +1840,182 @@
       <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="3:5">
       <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="10"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" ht="57.6" spans="2:5">
       <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="C10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" ht="86.4" spans="2:5">
       <c r="B11" s="6">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="C11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="6">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="C12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" ht="57.6" spans="2:5">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
+      <c r="C13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="C14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="2:5">
+      <c r="C15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" ht="72" spans="2:5">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="C16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
+      <c r="C18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="C19" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="6">
@@ -1861,7 +2085,7 @@
     </row>
     <row r="28" spans="3:5">
       <c r="C28" s="21" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="13"/>
@@ -1917,7 +2141,7 @@
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1946,7 +2170,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8"/>
       <c r="H4" s="6" t="s">
@@ -1964,7 +2188,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E5" s="20"/>
       <c r="H5" s="6" t="s">
@@ -1994,16 +2218,16 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -2199,7 +2423,7 @@
     </row>
     <row r="32" spans="3:5">
       <c r="C32" s="21" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="13"/>
@@ -2226,8 +2450,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4"/>
@@ -2256,7 +2480,7 @@
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2282,7 +2506,7 @@
     </row>
     <row r="4" spans="3:10">
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -2322,19 +2546,19 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -2551,7 +2775,7 @@
     </row>
     <row r="32" spans="3:6">
       <c r="C32" s="16" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>

</xml_diff>

<commit_message>
Refactoring plus Sonarlint - phase 1
</commit_message>
<xml_diff>
--- a/Tasks/Docs/CheckListsAll/Lab01_ReviewReport.xlsx
+++ b/Tasks/Docs/CheckListsAll/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\sem_5\VVSS2020\Tasks\Docs\CheckListsAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBC90FC-8CC8-4839-81BF-EFF8A9034D6D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C4FC70-E0D7-4689-9C55-00F25178A871}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9876" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22940" windowHeight="9880" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="123">
   <si>
     <t>do not print this form</t>
   </si>
@@ -300,18 +301,170 @@
   </si>
   <si>
     <t xml:space="preserve"> public ArrayTaskList(ArrayTaskList other)</t>
+  </si>
+  <si>
+    <t>protected ArrayTaskList clone()</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>TaskInfoController, 33</t>
+  </si>
+  <si>
+    <t>Perform check if an item is selected :       if(currentTask != null)</t>
+  </si>
+  <si>
+    <t>NewEditController, 112</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>NewEditController, 187</t>
+  </si>
+  <si>
+    <t>Use the error message return by the validation</t>
+  </si>
+  <si>
+    <t>TasksService, 44</t>
+  </si>
+  <si>
+    <t>C04, C08</t>
+  </si>
+  <si>
+    <t>Throw IllegalArgumentException if format is invalid</t>
+  </si>
+  <si>
+    <t>DateService, 36</t>
+  </si>
+  <si>
+    <t>DateService, 50</t>
+  </si>
+  <si>
+    <t>Tasks, 145</t>
+  </si>
+  <si>
+    <t>Add try - catch block</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>Outdated copies of elements are kept in different classes</t>
+  </si>
+  <si>
+    <t>TasksService, 18</t>
+  </si>
+  <si>
+    <t>Use ObservableList instead of TaskList</t>
+  </si>
+  <si>
+    <t>LinkedTasksList, 21</t>
+  </si>
+  <si>
+    <t>Fields in a "Serializable" class should either be transient or serializable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">private static class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Node</t>
+    </r>
+  </si>
+  <si>
+    <t>private static class Node implements Serializable</t>
+  </si>
+  <si>
+    <t>static base class members should not be accessed via derived types</t>
+  </si>
+  <si>
+    <t>DateService, 44</t>
+  </si>
+  <si>
+    <t>GregorianCalendar.getInstance()</t>
+  </si>
+  <si>
+    <r>
+      <t>java.util.Calendar.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>getInstance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Unused local variables should be removed</t>
+  </si>
+  <si>
+    <t>TaskRepository, 40</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>titleLength = dataInputStream.readInt()</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -381,6 +534,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCC7832"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF808080"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -482,88 +654,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -878,36 +1057,36 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="12.36328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="1"/>
     <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="14.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -931,10 +1110,10 @@
       <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
@@ -949,10 +1128,10 @@
       <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
@@ -968,19 +1147,19 @@
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="8" t="s">
@@ -996,7 +1175,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6">
+    <row r="10" spans="1:10" ht="58">
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -1010,7 +1189,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2">
+    <row r="11" spans="1:10" ht="43.5">
       <c r="B11" s="4">
         <f>B10+1</f>
         <v>2</v>
@@ -1043,7 +1222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8">
+    <row r="13" spans="1:10" ht="29">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1058,7 +1237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2">
+    <row r="14" spans="1:10" ht="43.5">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1073,7 +1252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8">
+    <row r="15" spans="1:10" ht="29">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1219,35 +1398,35 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="12.36328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="1"/>
     <col min="9" max="9" width="22" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -1271,10 +1450,10 @@
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1289,10 +1468,10 @@
       <c r="C5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1308,19 +1487,19 @@
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="8" t="s">
@@ -1336,7 +1515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6">
+    <row r="10" spans="1:10" ht="58">
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -1350,7 +1529,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="100.8">
+    <row r="11" spans="1:10" ht="101.5">
       <c r="B11" s="4">
         <f>B10+1</f>
         <v>2</v>
@@ -1380,7 +1559,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="57.6">
+    <row r="13" spans="1:10" ht="58">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1425,7 +1604,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72">
+    <row r="16" spans="1:10" ht="72.5">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1579,40 +1758,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="26.77734375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="12.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="1"/>
+    <col min="9" max="9" width="26.81640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -1636,10 +1815,10 @@
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1654,10 +1833,10 @@
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1673,15 +1852,15 @@
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="8" t="s">
@@ -1726,7 +1905,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8">
+    <row r="12" spans="1:10" ht="29">
       <c r="B12" s="4">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1758,8 +1937,14 @@
       <c r="D13" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="22" t="s">
         <v>85</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1777,77 +1962,125 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="29">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="C15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="C16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="29">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5">
+      <c r="C17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="29">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="C18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="29">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="2:5">
+      <c r="C19" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="29">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="C20" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="4">
@@ -1952,41 +2185,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="8.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="26.77734375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="8.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.54296875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.90625" style="1"/>
+    <col min="9" max="9" width="26.81640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
         <v>3</v>
@@ -2010,8 +2243,8 @@
       <c r="C4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
@@ -2026,8 +2259,8 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2043,8 +2276,8 @@
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="8" t="s">
@@ -2063,7 +2296,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" customHeight="1">
+    <row r="10" spans="1:10" ht="28.75" customHeight="1">
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -2073,19 +2306,19 @@
       <c r="D10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>91</v>
+      <c r="E10" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8">
+    <row r="11" spans="1:10" ht="29">
       <c r="B11" s="4">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="21" t="s">
@@ -2094,42 +2327,66 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="29">
       <c r="B12" s="4">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="C12" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="C13" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -2139,7 +2396,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2149,7 +2406,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -2159,7 +2416,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -2169,8 +2426,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
@@ -2179,7 +2436,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -2189,8 +2446,8 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
@@ -2199,7 +2456,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -2209,7 +2466,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -2219,7 +2476,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -2229,7 +2486,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -2239,8 +2496,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
@@ -2249,17 +2506,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -2269,7 +2526,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -2288,11 +2545,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="12"/>
     </row>
   </sheetData>

</xml_diff>